<commit_message>
improved change matrix spreadsheet
</commit_message>
<xml_diff>
--- a/documents/newton_raphson_change_matrix.xlsx
+++ b/documents/newton_raphson_change_matrix.xlsx
@@ -365,7 +365,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +658,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>F2*C8*SIN(E7-J2-E8)+G2*C9*SIN(E7-K2-E9)-2*E2*C7*SIN(I2)-C12*SIN(E7-E12)</f>
+        <f>(F2*C8*SIN(E7-J2-E8)+G2*C9*SIN(E7-K2-E9))-2*E2*C7*SIN(I2)-C12*SIN(E7-E12)</f>
         <v>-430.72216349844126</v>
       </c>
       <c r="B22">

</xml_diff>

<commit_message>
added another example to the spreadsheet
</commit_message>
<xml_diff>
--- a/documents/newton_raphson_change_matrix.xlsx
+++ b/documents/newton_raphson_change_matrix.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11265" windowHeight="7245"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11265" windowHeight="7245" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TwoPqAndOnePvNodeDifferentOrder" sheetId="1" r:id="rId1"/>
+    <sheet name="TwoPqNodes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
   <si>
     <t>currents</t>
   </si>
@@ -364,8 +365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,4 +704,211 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>COMPLEX(1, 2)</f>
+        <v>1+2i</v>
+      </c>
+      <c r="B2" t="str">
+        <f>COMPLEX(3, 4)</f>
+        <v>3+4i</v>
+      </c>
+      <c r="D2">
+        <f>IMABS(A2)</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="E2">
+        <f>IMABS(B2)</f>
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <f>IMARGUMENT(A2)</f>
+        <v>1.1071487177940904</v>
+      </c>
+      <c r="H2">
+        <f>IMARGUMENT(B2)</f>
+        <v>0.92729521800161219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>COMPLEX(5, 6)</f>
+        <v>5+6i</v>
+      </c>
+      <c r="B3" t="str">
+        <f>COMPLEX(7,8)</f>
+        <v>7+8i</v>
+      </c>
+      <c r="D3">
+        <f>IMABS(A3)</f>
+        <v>7.8102496759066558</v>
+      </c>
+      <c r="E3">
+        <f>IMABS(B3)</f>
+        <v>10.63014581273465</v>
+      </c>
+      <c r="G3">
+        <f>IMARGUMENT(A3)</f>
+        <v>0.87605805059819342</v>
+      </c>
+      <c r="H3">
+        <f>IMARGUMENT(B3)</f>
+        <v>0.85196632717327203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>COMPLEX(9,10)</f>
+        <v>9+10i</v>
+      </c>
+      <c r="C6">
+        <f>IMABS(A6)</f>
+        <v>13.453624047073712</v>
+      </c>
+      <c r="E6">
+        <f>IMARGUMENT(A6)</f>
+        <v>0.83798122500839001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>COMPLEX(11,12)</f>
+        <v>11+12i</v>
+      </c>
+      <c r="C7">
+        <f>IMABS(A7)</f>
+        <v>16.278820596099706</v>
+      </c>
+      <c r="E7">
+        <f>IMARGUMENT(A7)</f>
+        <v>0.82884905878897908</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>COMPLEX(13,14)</f>
+        <v>13+14i</v>
+      </c>
+      <c r="C10">
+        <f>IMABS(A10)</f>
+        <v>19.104973174542799</v>
+      </c>
+      <c r="E10">
+        <f>IMARGUMENT(A10)</f>
+        <v>0.82241827927137834</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>COMPLEX(15,16)</f>
+        <v>15+16i</v>
+      </c>
+      <c r="C11">
+        <f>IMABS(A11)</f>
+        <v>21.931712199461309</v>
+      </c>
+      <c r="E11">
+        <f>IMARGUMENT(A11)</f>
+        <v>0.81764504583270226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>-C6*E2*C7*SIN(E6-H2-E7)+C10*C6*SIN(E6-E10)</f>
+        <v>873.99999999999989</v>
+      </c>
+      <c r="B14">
+        <f>C6*E2*C7*SIN(E6-H2-E7)</f>
+        <v>-869.99999999999989</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>C6*D3*C7*SIN(E7-G3-E6)</f>
+        <v>-1324.0000000000005</v>
+      </c>
+      <c r="B15">
+        <f>-C7*D3*C6*SIN(E7-G3-E6)+C11*C7*SIN(E7-E11)</f>
+        <v>1328.0000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f>E2*C7*SIN(E6-H2-E7)-2*D2*C6*SIN(G2)-C10*SIN(E6-E10)</f>
+        <v>-118.77840457029718</v>
+      </c>
+      <c r="B18">
+        <f>C6*E2*SIN(E6-H2-E7)</f>
+        <v>-53.443675164553753</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>C7*D3*SIN(E7-G3-E6)</f>
+        <v>-98.412144963124845</v>
+      </c>
+      <c r="B19">
+        <f>D3*C6*SIN(E7-G3-E6)-2*E3*C7*SIN(H3)-C11*SIN(E7-E11)</f>
+        <v>-342.03952105314409</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
extended spreadsheet for change matrices
</commit_message>
<xml_diff>
--- a/documents/newton_raphson_change_matrix.xlsx
+++ b/documents/newton_raphson_change_matrix.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benediktibk\Entwicklung\Loadflow\dev\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benedikt\Entwicklung\LoadFlow\dev\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11265" windowHeight="7245"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11265" windowHeight="7245" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TwoPqAndOnePvNodeDifferentOrder" sheetId="1" r:id="rId1"/>
     <sheet name="TwoPqNodes" sheetId="2" r:id="rId2"/>
+    <sheet name="ThreePqNodes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>currents</t>
   </si>
@@ -46,6 +47,36 @@
   </si>
   <si>
     <t>imaginary power by amplitude</t>
+  </si>
+  <si>
+    <t>admittances, real</t>
+  </si>
+  <si>
+    <t>admittances, imaginary</t>
+  </si>
+  <si>
+    <t>voltages, real</t>
+  </si>
+  <si>
+    <t>voltages, imaginary</t>
+  </si>
+  <si>
+    <t>currents, real</t>
+  </si>
+  <si>
+    <t>currents, imaginary</t>
+  </si>
+  <si>
+    <t>real power by real</t>
+  </si>
+  <si>
+    <t>real power by imaginary</t>
+  </si>
+  <si>
+    <t>imaginary power by real</t>
+  </si>
+  <si>
+    <t>imaginary power by imaginary</t>
   </si>
 </sst>
 </file>
@@ -53,7 +84,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -86,7 +117,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,7 +400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
@@ -937,4 +968,323 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>27</v>
+      </c>
+      <c r="C13">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>(B2*$A8-F2*$C8)+(C2*$A9-G2*$C9)+2*A2*$A7-$A12</f>
+        <v>-41</v>
+      </c>
+      <c r="B17">
+        <f>A7*B2+C7*F2</f>
+        <v>137</v>
+      </c>
+      <c r="C17">
+        <f>A7*C2+C7*G2</f>
+        <v>215</v>
+      </c>
+      <c r="E17">
+        <f>(F2*A8+B2*C8)+(G2*A9+C2*C9)+2*A2*C7-C12</f>
+        <v>422</v>
+      </c>
+      <c r="F17">
+        <f>$C7*B2-$A7*F2</f>
+        <v>-16</v>
+      </c>
+      <c r="G17">
+        <f>$C7*C2-$A7*G2</f>
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f>A8*A3+C8*E3</f>
+        <v>323</v>
+      </c>
+      <c r="B18">
+        <f>(A3*A7-E3*C7)+(C3*A9-G3*C9)+2*B3*A8-A13</f>
+        <v>289</v>
+      </c>
+      <c r="C18">
+        <f>A8*C3+C8*G3</f>
+        <v>495</v>
+      </c>
+      <c r="E18">
+        <f>$C8*A3-$A8*E3</f>
+        <v>-14</v>
+      </c>
+      <c r="F18">
+        <f>(E3*A7+A3*C7)+(G3*A9+C3*C9)+2*B3*C8-C13</f>
+        <v>1200</v>
+      </c>
+      <c r="G18">
+        <f>$C8*C3-$A8*G3</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>A9*A4+C9*E4</f>
+        <v>635</v>
+      </c>
+      <c r="B19">
+        <f>A9*B4+C9*F4</f>
+        <v>729</v>
+      </c>
+      <c r="C19">
+        <f>(A4*A7-E4*C7)+(B4*A8-F4*C8)+2*C4*A9-A14</f>
+        <v>683</v>
+      </c>
+      <c r="E19">
+        <f>$C9*A4-$A9*E4</f>
+        <v>-10</v>
+      </c>
+      <c r="F19">
+        <f>$C9*B4-$A9*F4</f>
+        <v>-8</v>
+      </c>
+      <c r="G19">
+        <f>(E4*A7+A4*C7)+(F4*A8+B4*C8)+2*C4*C9-C14</f>
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>(-F2*A8-B2*C8)+(-G2*A9-C2*C9)-2*E2*A7-C12</f>
+        <v>-510</v>
+      </c>
+      <c r="B22">
+        <f>$C7*B2-$A7*F2</f>
+        <v>-16</v>
+      </c>
+      <c r="C22">
+        <f>$C7*C2-$A7*G2</f>
+        <v>-14</v>
+      </c>
+      <c r="E22">
+        <f>(B2*A8-F2*C8)+(C2*A9-G2*C9)-2*E2*C7+A12</f>
+        <v>-109</v>
+      </c>
+      <c r="F22">
+        <f>-$A7*B2-$C7*F2</f>
+        <v>-137</v>
+      </c>
+      <c r="G22">
+        <f>-$A7*C2-$C7*G2</f>
+        <v>-215</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>$C8*A3-$A8*E3</f>
+        <v>-14</v>
+      </c>
+      <c r="B23">
+        <f>(-E3*A7-A3*C7)+(-G3*A9-C3*C9)-2*F3*A8-C13</f>
+        <v>-1280</v>
+      </c>
+      <c r="C23">
+        <f>$C8*C3-$A8*G3</f>
+        <v>-10</v>
+      </c>
+      <c r="E23">
+        <f>-$A8*A3-$C8*E3</f>
+        <v>-323</v>
+      </c>
+      <c r="F23">
+        <f>(A3*A7-E3*C7)+(C3*A9-G3*C9)-2*F3*C8+A13</f>
+        <v>-475</v>
+      </c>
+      <c r="G23">
+        <f>-$A8*C3-$C8*G3</f>
+        <v>-495</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f>$C9*A4-$A9*E4</f>
+        <v>-10</v>
+      </c>
+      <c r="B24">
+        <f>$C9*B4-$A9*F4</f>
+        <v>-8</v>
+      </c>
+      <c r="C24">
+        <f>(-E4*A7-A4*C7)+(-F4*A8-B4*C8)-2*G4*A9-C14</f>
+        <v>-2050</v>
+      </c>
+      <c r="E24">
+        <f>-$A9*A4-$C9*E4</f>
+        <v>-635</v>
+      </c>
+      <c r="F24">
+        <f>-$A9*B4-$C9*F4</f>
+        <v>-729</v>
+      </c>
+      <c r="G24">
+        <f>(A4*A7-E4*C7)+(B4*A8-F4*C8)-2*G4*C9+A14</f>
+        <v>-905</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed error in formula
</commit_message>
<xml_diff>
--- a/documents/newton_raphson_change_matrix.xlsx
+++ b/documents/newton_raphson_change_matrix.xlsx
@@ -975,7 +975,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,8 +1232,8 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>(-F2*A8-B2*C8)+(-G2*A9-C2*C9)-2*E2*A7-C12</f>
-        <v>-510</v>
+        <f>(-F2*A8-B2*C8)+(-G2*A9-C2*C9)-2*E2*A7+C12</f>
+        <v>-458</v>
       </c>
       <c r="B22">
         <f>$C7*B2-$A7*F2</f>
@@ -1244,8 +1244,8 @@
         <v>-14</v>
       </c>
       <c r="E22">
-        <f>(B2*A8-F2*C8)+(C2*A9-G2*C9)-2*E2*C7+A12</f>
-        <v>-109</v>
+        <f>(B2*A8-F2*C8)+(C2*A9-G2*C9)-2*E2*C7-A12</f>
+        <v>-159</v>
       </c>
       <c r="F22">
         <f>-$A7*B2-$C7*F2</f>
@@ -1262,8 +1262,8 @@
         <v>-14</v>
       </c>
       <c r="B23">
-        <f>(-E3*A7-A3*C7)+(-G3*A9-C3*C9)-2*F3*A8-C13</f>
-        <v>-1280</v>
+        <f>(-E3*A7-A3*C7)+(-G3*A9-C3*C9)-2*F3*A8+C13</f>
+        <v>-1224</v>
       </c>
       <c r="C23">
         <f>$C8*C3-$A8*G3</f>
@@ -1274,8 +1274,8 @@
         <v>-323</v>
       </c>
       <c r="F23">
-        <f>(A3*A7-E3*C7)+(C3*A9-G3*C9)-2*F3*C8+A13</f>
-        <v>-475</v>
+        <f>(A3*A7-E3*C7)+(C3*A9-G3*C9)-2*F3*C8-A13</f>
+        <v>-529</v>
       </c>
       <c r="G23">
         <f>-$A8*C3-$C8*G3</f>
@@ -1292,8 +1292,8 @@
         <v>-8</v>
       </c>
       <c r="C24">
-        <f>(-E4*A7-A4*C7)+(-F4*A8-B4*C8)-2*G4*A9-C14</f>
-        <v>-2050</v>
+        <f>(-E4*A7-A4*C7)+(-F4*A8-B4*C8)-2*G4*A9+C14</f>
+        <v>-1990</v>
       </c>
       <c r="E24">
         <f>-$A9*A4-$C9*E4</f>
@@ -1304,8 +1304,8 @@
         <v>-729</v>
       </c>
       <c r="G24">
-        <f>(A4*A7-E4*C7)+(B4*A8-F4*C8)-2*G4*C9+A14</f>
-        <v>-905</v>
+        <f>(A4*A7-E4*C7)+(B4*A8-F4*C8)-2*G4*C9-A14</f>
+        <v>-963</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tried to fix change matrix
</commit_message>
<xml_diff>
--- a/documents/newton_raphson_change_matrix.xlsx
+++ b/documents/newton_raphson_change_matrix.xlsx
@@ -105,12 +105,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -125,9 +131,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1328,7 +1336,7 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,7 +1738,7 @@
         <f>$I7*N2-$G7*R2</f>
         <v>-16</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <f>C7*G2*C9*SIN(E7-K2-E9)</f>
         <v>-5482.0000000000009</v>
       </c>
@@ -1786,15 +1794,15 @@
         <f>$G9*N4+$I9*R4</f>
         <v>729</v>
       </c>
-      <c r="D19">
-        <f>$I9*M4-$G9*Q4</f>
+      <c r="D19" s="3">
+        <f>$I$9*$M$4-$G$9*$Q$4</f>
         <v>-10</v>
       </c>
       <c r="E19">
         <f>$I9*N4-$G9*R4</f>
         <v>-8</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <f>-(C9*E4*C7*SIN(E9-I4-E7)+C9*F4*C8*SIN(E9-J4-E8))+C14*C9*SIN(E9-E14)</f>
         <v>29102</v>
       </c>
@@ -1827,7 +1835,7 @@
         <f>-$G7*N2-$I7*R2</f>
         <v>-137</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2">
         <f>-C7*G2*C9*COS(E7-K2-E9)</f>
         <v>-4609</v>
       </c>

</xml_diff>

<commit_message>
fixed error in calculation of change matrix
</commit_message>
<xml_diff>
--- a/documents/newton_raphson_change_matrix.xlsx
+++ b/documents/newton_raphson_change_matrix.xlsx
@@ -1336,7 +1336,7 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,7 +1738,7 @@
         <f>$I7*N2-$G7*R2</f>
         <v>-16</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="3">
         <f>C7*G2*C9*SIN(E7-K2-E9)</f>
         <v>-5482.0000000000009</v>
       </c>

</xml_diff>

<commit_message>
added test for calculation of change matrix
</commit_message>
<xml_diff>
--- a/documents/newton_raphson_change_matrix.xlsx
+++ b/documents/newton_raphson_change_matrix.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benedikt\Entwicklung\LoadFlow\dev\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benediktibk\Entwicklung\Loadflow\dev\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11265" windowHeight="7245" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11265" windowHeight="7245" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TwoPqAndOnePvNodeDifferentOrder" sheetId="1" r:id="rId1"/>
     <sheet name="TwoPqNodes" sheetId="2" r:id="rId2"/>
     <sheet name="ThreePqNodes" sheetId="3" r:id="rId3"/>
     <sheet name="TwoPqAndOnePvNodeDifferentOrde2" sheetId="4" r:id="rId4"/>
+    <sheet name="OnePvAndOnePqNode" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="26">
   <si>
     <t>currents</t>
   </si>
@@ -87,6 +88,24 @@
   </si>
   <si>
     <t>imaginary power by angle</t>
+  </si>
+  <si>
+    <t>magnitude</t>
+  </si>
+  <si>
+    <t>phase</t>
+  </si>
+  <si>
+    <t>real power by real part</t>
+  </si>
+  <si>
+    <t>real power by imaginary part</t>
+  </si>
+  <si>
+    <t>imaginary power by real part</t>
+  </si>
+  <si>
+    <t>imaginary power by imaginary part</t>
   </si>
 </sst>
 </file>
@@ -131,11 +150,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1335,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,10 +1851,6 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f>(-R2*G8-N2*I8)+(-S2*G9-O2*I9)-2*Q2*G7+I12</f>
-        <v>-458</v>
-      </c>
       <c r="B22">
         <f>$I7*N2-$G7*R2</f>
         <v>-16</v>
@@ -1853,10 +1869,6 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f>$I8*M3-$G8*Q3</f>
-        <v>-14</v>
-      </c>
       <c r="B23">
         <f>(-Q3*G7-M3*I7)+(-S3*G9-O3*I9)-2*R3*G8+I13</f>
         <v>-1224</v>
@@ -1872,6 +1884,309 @@
       <c r="G23">
         <f>-C8*G3*C9*COS(E8-K3-E9)</f>
         <v>-11145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>COMPLEX(0.6, -0.6)</f>
+        <v>0,6-0,6i</v>
+      </c>
+      <c r="B2" t="str">
+        <f>COMPLEX(-0.2, 0.4)</f>
+        <v>-0,2+0,4i</v>
+      </c>
+      <c r="D2">
+        <f>IMREAL(A2)</f>
+        <v>0.6</v>
+      </c>
+      <c r="E2">
+        <f>IMREAL(B2)</f>
+        <v>-0.2</v>
+      </c>
+      <c r="G2">
+        <f>IMAGINARY(A2)</f>
+        <v>-0.6</v>
+      </c>
+      <c r="H2">
+        <f>IMAGINARY(B2)</f>
+        <v>0.4</v>
+      </c>
+      <c r="J2">
+        <f>IMABS(A2)</f>
+        <v>0.84852813742385702</v>
+      </c>
+      <c r="K2">
+        <f>IMABS(B2)</f>
+        <v>0.44721359549995798</v>
+      </c>
+      <c r="M2">
+        <f>IMARGUMENT(A2)</f>
+        <v>-0.78539816339744828</v>
+      </c>
+      <c r="N2">
+        <f>IMARGUMENT(B2)</f>
+        <v>2.0344439357957027</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>COMPLEX(-0.2,0.4)</f>
+        <v>-0,2+0,4i</v>
+      </c>
+      <c r="B3" t="str">
+        <f>COMPLEX(0.2,-0.4)</f>
+        <v>0,2-0,4i</v>
+      </c>
+      <c r="D3">
+        <f>IMREAL(A3)</f>
+        <v>-0.2</v>
+      </c>
+      <c r="E3">
+        <f>IMREAL(B3)</f>
+        <v>0.2</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G4" si="0">IMAGINARY(A3)</f>
+        <v>0.4</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H4" si="1">IMAGINARY(B3)</f>
+        <v>-0.4</v>
+      </c>
+      <c r="J3">
+        <f>IMABS(A3)</f>
+        <v>0.44721359549995798</v>
+      </c>
+      <c r="K3">
+        <f>IMABS(B3)</f>
+        <v>0.44721359549995798</v>
+      </c>
+      <c r="M3">
+        <f>IMARGUMENT(A3)</f>
+        <v>2.0344439357957027</v>
+      </c>
+      <c r="N3">
+        <f>IMARGUMENT(B3)</f>
+        <v>-1.1071487177940904</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>COMPLEX(10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <f>IMREAL(A6)</f>
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <f>IMAGINARY(A6)</f>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f>IMABS(A6)</f>
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <f>IMARGUMENT(A6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>COMPLEX(10,0)</f>
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <f>IMREAL(A7)</f>
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <f>IMAGINARY(A7)</f>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f>IMABS(A7)</f>
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <f>IMARGUMENT(A7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>COMPLEX(4.02,-1.96)</f>
+        <v>4,02-1,96i</v>
+      </c>
+      <c r="C10">
+        <f>IMREAL(A10)</f>
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="E10">
+        <f>IMAGINARY(A10)</f>
+        <v>-1.96</v>
+      </c>
+      <c r="G10">
+        <f>IMABS(A10)</f>
+        <v>4.4723595562074383</v>
+      </c>
+      <c r="I10">
+        <f>IMARGUMENT(A10)</f>
+        <v>-0.45364794231414091</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>COMPLEX(0,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <f>IMREAL(A11)</f>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f>IMAGINARY(A11)</f>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f>IMABS(A11)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" t="e">
+        <f>IMARGUMENT(A11)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <f>E2*C7+2*D2*C6-C10</f>
+        <v>5.98</v>
+      </c>
+      <c r="E14">
+        <f>H2*C7-E10</f>
+        <v>5.96</v>
+      </c>
+      <c r="I14">
+        <f>G6*K2*G7*SIN(-N2)</f>
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>C7*D3</f>
+        <v>-2</v>
+      </c>
+      <c r="E15">
+        <f>-C7*G3</f>
+        <v>-4</v>
+      </c>
+      <c r="I15">
+        <f>C7*J3*C6*SIN(-M3)</f>
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f>-H2*C7-2*G2*C6+E10</f>
+        <v>6.04</v>
+      </c>
+      <c r="E18">
+        <f>E2*C7-C10</f>
+        <v>-6.02</v>
+      </c>
+      <c r="I18">
+        <f>-C6*K2*C7*COS(-N2)</f>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>